<commit_message>
added cell color changing to red when tomato amount was too large and user can now enter file name
</commit_message>
<xml_diff>
--- a/testFile.xlsx
+++ b/testFile.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -27,12 +27,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -47,10 +53,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -498,7 +505,56 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n"/>
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>11/18/2022 20:50:36</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>107</v>
+      </c>
+      <c r="C5" t="n">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>11/18/2022 21:20:03</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>150</v>
+      </c>
+      <c r="C6" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>11/18/2022 21:24:51</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>110</v>
+      </c>
+      <c r="C7" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>11/18/2022 21:27:11</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>115</v>
+      </c>
+      <c r="C8" t="n">
+        <v>115</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>